<commit_message>
Change ASB to MCSB
</commit_message>
<xml_diff>
--- a/ready/Azure Security Control Mapping- Template with Example.xlsx
+++ b/ready/Azure Security Control Mapping- Template with Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/tanshah_microsoft_com/Documents/Control mappings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\CloudAdoptionFramework\ready\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{1D01736C-CDAD-4421-9F10-177595EC18C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA86A57A-C30B-452F-BDD5-C27F1DD00D24}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DEC078-9658-42B7-B754-C20BDED5CE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="3555" windowWidth="19515" windowHeight="10433" firstSheet="1" activeTab="1" xr2:uid="{397B3869-B272-4315-9061-FF6A0CE2DF8F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="1" xr2:uid="{397B3869-B272-4315-9061-FF6A0CE2DF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Contoso Controls" sheetId="1" r:id="rId1"/>
@@ -120,15 +120,6 @@
     <t>Contoso Cloud Security Requirement</t>
   </si>
   <si>
-    <t>ASB Mapping</t>
-  </si>
-  <si>
-    <t>ASB Guidance</t>
-  </si>
-  <si>
-    <t>ASB Policy</t>
-  </si>
-  <si>
     <t>Relevant Azure Security Baseline</t>
   </si>
   <si>
@@ -309,6 +300,15 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>MCSB Mapping</t>
+  </si>
+  <si>
+    <t>MCSB Guidance</t>
+  </si>
+  <si>
+    <t>MCSB Policy</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1149,7 @@
   <sheetViews>
     <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B6"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1235,36 +1235,36 @@
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>11</v>
       </c>
       <c r="K3" s="13"/>
       <c r="L3" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N3" s="13"/>
       <c r="O3" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Q3" s="29"/>
     </row>
     <row r="4" spans="1:17" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="48" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="48"/>
       <c r="D4" s="48"/>
@@ -1273,46 +1273,46 @@
     </row>
     <row r="5" spans="1:17" ht="220.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="E5" s="45" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>21</v>
       </c>
       <c r="F5" s="30"/>
       <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="K5" s="30"/>
       <c r="L5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N5" s="30"/>
       <c r="O5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q5" s="25"/>
     </row>
@@ -1324,28 +1324,28 @@
       <c r="E6" s="45"/>
       <c r="F6" s="30"/>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="30"/>
       <c r="L6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="N6" s="30"/>
       <c r="O6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q6" s="25"/>
     </row>
@@ -1370,89 +1370,89 @@
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="E8" s="17" t="s">
         <v>35</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>38</v>
       </c>
       <c r="F8" s="30"/>
       <c r="G8" s="38" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K8" s="30"/>
       <c r="L8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N8" s="30"/>
       <c r="O8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="Q8" s="14"/>
     </row>
     <row r="9" spans="1:17" ht="117" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="41"/>
       <c r="B9" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D9" s="8">
         <v>12.5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F9" s="30"/>
       <c r="G9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K9" s="30"/>
       <c r="L9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N9" s="30"/>
       <c r="O9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="Q9" s="25"/>
     </row>
@@ -1470,7 +1470,7 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B4:E4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C9 E9 B5:C5 B8:E8">
+  <conditionalFormatting sqref="B5:C5 B8:E8 E9">
     <cfRule type="expression" dxfId="5" priority="8">
       <formula>#REF!="Remove TSF"</formula>
     </cfRule>
@@ -1498,9 +1498,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A99D0F0-3E51-49EB-9839-EB12A6CF5B57}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7:O7"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1526,7 +1526,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="14.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="44" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -1558,7 +1558,7 @@
       <c r="I2" s="28"/>
       <c r="J2" s="25"/>
       <c r="K2" s="43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L2" s="43"/>
       <c r="M2" s="27"/>
@@ -1570,49 +1570,49 @@
     </row>
     <row r="3" spans="1:16" s="6" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>11</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="M3" s="13"/>
       <c r="N3" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="P3" s="29"/>
     </row>
     <row r="4" spans="1:16" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="48" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
@@ -1621,43 +1621,43 @@
     </row>
     <row r="5" spans="1:16" ht="220.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="45" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>21</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="J5" s="30"/>
       <c r="K5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M5" s="30"/>
       <c r="N5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P5" s="25"/>
     </row>
@@ -1668,28 +1668,28 @@
       <c r="D6" s="45"/>
       <c r="E6" s="30"/>
       <c r="F6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="30"/>
       <c r="K6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M6" s="30"/>
       <c r="N6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P6" s="25"/>
     </row>
@@ -1735,7 +1735,7 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B8 D8 A5:B5 A7:D7">
+  <conditionalFormatting sqref="A5:B5 A7:D7 B8 D8">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>#REF!="Remove TSF"</formula>
     </cfRule>
@@ -1759,6 +1759,43 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Story_x0020_Type xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466">
+      <Value>Production Release</Value>
+    </Story_x0020_Type>
+    <AIService xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
+    <Customer xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
+    <Classification xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
+    <Segment xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
+    <Industry xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
+    <SharedWithUsers xmlns="fc000d47-5a8d-4c17-93da-7dc36117dfec">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A243BABB20851846966C94EEE12FE7C5" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="894bf12bf4fc228a272e86e19c737f5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fc000d47-5a8d-4c17-93da-7dc36117dfec" xmlns:ns3="b6cd650e-13f9-4068-89e6-ce32be2a5466" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb91b9a3e29cd865c3f96be23fb2c0ac" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2095,44 +2132,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F7FDE82-95B4-4F72-9E1E-7C3B63F42775}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b6cd650e-13f9-4068-89e6-ce32be2a5466"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fc000d47-5a8d-4c17-93da-7dc36117dfec"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Story_x0020_Type xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466">
-      <Value>Production Release</Value>
-    </Story_x0020_Type>
-    <AIService xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
-    <Customer xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
-    <Classification xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
-    <Segment xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
-    <Industry xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
-    <SharedWithUsers xmlns="fc000d47-5a8d-4c17-93da-7dc36117dfec">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0485DD06-A2A0-45BF-ACE3-E7C1D95FEBB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{234268D5-B664-429F-90D7-836B0A8866DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2153,33 +2180,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0485DD06-A2A0-45BF-ACE3-E7C1D95FEBB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F7FDE82-95B4-4F72-9E1E-7C3B63F42775}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b6cd650e-13f9-4068-89e6-ce32be2a5466"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fc000d47-5a8d-4c17-93da-7dc36117dfec"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
Change ASB to MCSB (#117)
</commit_message>
<xml_diff>
--- a/ready/Azure Security Control Mapping- Template with Example.xlsx
+++ b/ready/Azure Security Control Mapping- Template with Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/tanshah_microsoft_com/Documents/Control mappings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\CloudAdoptionFramework\ready\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{1D01736C-CDAD-4421-9F10-177595EC18C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA86A57A-C30B-452F-BDD5-C27F1DD00D24}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DEC078-9658-42B7-B754-C20BDED5CE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="3555" windowWidth="19515" windowHeight="10433" firstSheet="1" activeTab="1" xr2:uid="{397B3869-B272-4315-9061-FF6A0CE2DF8F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="1" xr2:uid="{397B3869-B272-4315-9061-FF6A0CE2DF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Contoso Controls" sheetId="1" r:id="rId1"/>
@@ -120,15 +120,6 @@
     <t>Contoso Cloud Security Requirement</t>
   </si>
   <si>
-    <t>ASB Mapping</t>
-  </si>
-  <si>
-    <t>ASB Guidance</t>
-  </si>
-  <si>
-    <t>ASB Policy</t>
-  </si>
-  <si>
     <t>Relevant Azure Security Baseline</t>
   </si>
   <si>
@@ -309,6 +300,15 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>MCSB Mapping</t>
+  </si>
+  <si>
+    <t>MCSB Guidance</t>
+  </si>
+  <si>
+    <t>MCSB Policy</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1149,7 @@
   <sheetViews>
     <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B6"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1235,36 +1235,36 @@
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>11</v>
       </c>
       <c r="K3" s="13"/>
       <c r="L3" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N3" s="13"/>
       <c r="O3" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Q3" s="29"/>
     </row>
     <row r="4" spans="1:17" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="48" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="48"/>
       <c r="D4" s="48"/>
@@ -1273,46 +1273,46 @@
     </row>
     <row r="5" spans="1:17" ht="220.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="E5" s="45" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>21</v>
       </c>
       <c r="F5" s="30"/>
       <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="K5" s="30"/>
       <c r="L5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N5" s="30"/>
       <c r="O5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q5" s="25"/>
     </row>
@@ -1324,28 +1324,28 @@
       <c r="E6" s="45"/>
       <c r="F6" s="30"/>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="30"/>
       <c r="L6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="N6" s="30"/>
       <c r="O6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q6" s="25"/>
     </row>
@@ -1370,89 +1370,89 @@
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="E8" s="17" t="s">
         <v>35</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>38</v>
       </c>
       <c r="F8" s="30"/>
       <c r="G8" s="38" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K8" s="30"/>
       <c r="L8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N8" s="30"/>
       <c r="O8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P8" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="Q8" s="14"/>
     </row>
     <row r="9" spans="1:17" ht="117" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="41"/>
       <c r="B9" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D9" s="8">
         <v>12.5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F9" s="30"/>
       <c r="G9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K9" s="30"/>
       <c r="L9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N9" s="30"/>
       <c r="O9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P9" s="38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="Q9" s="25"/>
     </row>
@@ -1470,7 +1470,7 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B4:E4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C9 E9 B5:C5 B8:E8">
+  <conditionalFormatting sqref="B5:C5 B8:E8 E9">
     <cfRule type="expression" dxfId="5" priority="8">
       <formula>#REF!="Remove TSF"</formula>
     </cfRule>
@@ -1498,9 +1498,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A99D0F0-3E51-49EB-9839-EB12A6CF5B57}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7:O7"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1526,7 +1526,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="14.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="44" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -1558,7 +1558,7 @@
       <c r="I2" s="28"/>
       <c r="J2" s="25"/>
       <c r="K2" s="43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L2" s="43"/>
       <c r="M2" s="27"/>
@@ -1570,49 +1570,49 @@
     </row>
     <row r="3" spans="1:16" s="6" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>11</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="M3" s="13"/>
       <c r="N3" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="P3" s="29"/>
     </row>
     <row r="4" spans="1:16" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="48" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
@@ -1621,43 +1621,43 @@
     </row>
     <row r="5" spans="1:16" ht="220.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="45" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>21</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="J5" s="30"/>
       <c r="K5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M5" s="30"/>
       <c r="N5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P5" s="25"/>
     </row>
@@ -1668,28 +1668,28 @@
       <c r="D6" s="45"/>
       <c r="E6" s="30"/>
       <c r="F6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="30"/>
       <c r="K6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M6" s="30"/>
       <c r="N6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P6" s="25"/>
     </row>
@@ -1735,7 +1735,7 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B8 D8 A5:B5 A7:D7">
+  <conditionalFormatting sqref="A5:B5 A7:D7 B8 D8">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>#REF!="Remove TSF"</formula>
     </cfRule>
@@ -1759,6 +1759,43 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Story_x0020_Type xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466">
+      <Value>Production Release</Value>
+    </Story_x0020_Type>
+    <AIService xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
+    <Customer xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
+    <Classification xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
+    <Segment xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
+    <Industry xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
+    <SharedWithUsers xmlns="fc000d47-5a8d-4c17-93da-7dc36117dfec">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A243BABB20851846966C94EEE12FE7C5" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="894bf12bf4fc228a272e86e19c737f5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fc000d47-5a8d-4c17-93da-7dc36117dfec" xmlns:ns3="b6cd650e-13f9-4068-89e6-ce32be2a5466" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb91b9a3e29cd865c3f96be23fb2c0ac" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2095,44 +2132,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F7FDE82-95B4-4F72-9E1E-7C3B63F42775}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b6cd650e-13f9-4068-89e6-ce32be2a5466"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fc000d47-5a8d-4c17-93da-7dc36117dfec"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Story_x0020_Type xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466">
-      <Value>Production Release</Value>
-    </Story_x0020_Type>
-    <AIService xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
-    <Customer xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
-    <Classification xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
-    <Segment xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
-    <Industry xmlns="b6cd650e-13f9-4068-89e6-ce32be2a5466" xsi:nil="true"/>
-    <SharedWithUsers xmlns="fc000d47-5a8d-4c17-93da-7dc36117dfec">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0485DD06-A2A0-45BF-ACE3-E7C1D95FEBB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{234268D5-B664-429F-90D7-836B0A8866DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2153,33 +2180,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0485DD06-A2A0-45BF-ACE3-E7C1D95FEBB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F7FDE82-95B4-4F72-9E1E-7C3B63F42775}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b6cd650e-13f9-4068-89e6-ce32be2a5466"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fc000d47-5a8d-4c17-93da-7dc36117dfec"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>